<commit_message>
Fixed vertical bundle and missing SKU text formatting
</commit_message>
<xml_diff>
--- a/data_jul4/SO-PackExport Data_1013582.xlsx
+++ b/data_jul4/SO-PackExport Data_1013582.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\Source\bundle-optimization-new\data_jul4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40179424-9D92-4B22-8C5E-F9FA2FA5260A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8589E915-E10C-4473-9475-66E40ACC9F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,7 +567,7 @@
   <dimension ref="A1:AP146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -760,7 +760,9 @@
       <c r="E2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2">
+        <v>2</v>
+      </c>
       <c r="G2" s="2" t="s">
         <v>61</v>
       </c>
@@ -879,7 +881,9 @@
       <c r="E3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
       <c r="G3" s="2" t="s">
         <v>70</v>
       </c>
@@ -998,7 +1002,9 @@
       <c r="E4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
       <c r="G4" s="2" t="s">
         <v>72</v>
       </c>
@@ -1117,7 +1123,9 @@
       <c r="E5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
       <c r="G5" s="2" t="s">
         <v>74</v>
       </c>
@@ -1236,7 +1244,9 @@
       <c r="E6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
       <c r="G6" s="2" t="s">
         <v>76</v>
       </c>
@@ -1355,7 +1365,9 @@
       <c r="E7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
       <c r="G7" s="2" t="s">
         <v>78</v>
       </c>
@@ -1474,7 +1486,9 @@
       <c r="E8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
       <c r="G8" s="2" t="s">
         <v>55</v>
       </c>
@@ -1593,7 +1607,9 @@
       <c r="E9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2">
+        <v>2</v>
+      </c>
       <c r="G9" s="2" t="s">
         <v>57</v>
       </c>
@@ -1712,7 +1728,9 @@
       <c r="E10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2">
+        <v>2</v>
+      </c>
       <c r="G10" s="2" t="s">
         <v>80</v>
       </c>

</xml_diff>